<commit_message>
updated with Vishal and Zahoor version
</commit_message>
<xml_diff>
--- a/instructions/Users.xlsx
+++ b/instructions/Users.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29003"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29519"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisdem\Downloads\SendPromotion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoftapc.sharepoint.com/teams/CopilotChat-IndiaRollout/Shared Documents/Reference Materials/Nudges - Copilot chat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B831F965-7387-4BA5-ADAD-FE14FAD2AF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{DCDF6BA5-0396-4DDC-887B-897A379A886D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2376C2AC-634D-46CA-95A8-69B756557C05}"/>
   <bookViews>
-    <workbookView xWindow="35880" yWindow="4710" windowWidth="29040" windowHeight="15720" xr2:uid="{E2CFDE0D-5E57-4304-85AB-0C475CA40F4A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{E2CFDE0D-5E57-4304-85AB-0C475CA40F4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,25 +36,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>UPN</t>
   </si>
   <si>
-    <t>AmberR@M365CPI69113837.OnMicrosoft.com</t>
-  </si>
-  <si>
-    <t>BillieV@M365CPI69113837.OnMicrosoft.com</t>
-  </si>
-  <si>
-    <t>admin@M365CPI69113837.onmicrosoft.com</t>
+    <t>AmberR@M365CPI14039056.OnMicrosoft.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,70 +436,70 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="48.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1">
       <c r="A14" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{DCB587C1-2EE2-4C9D-935D-BAF6489B8310}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{1ED7D2F8-8E75-4EE7-B2C9-CA96D3BFCDA8}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{DC5F3F85-A2F3-45FB-BA08-359B9B7DB563}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C1D66C95E8B086489DD3BAFD8DB2FD77" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bd21b9be05c2766d5b74d77f00fdda2c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="5a827679-a132-4c88-bdb0-a978ce7a8b2d" xmlns:ns3="9921d756-3b1e-4e19-bd90-0d5dcbdf1ae1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fbf117d8d43c584bb1266341db86766a" ns1:_="" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B937F5FCAF8B62499A2D7BF1F8F85E44" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d16c9c73fc3e3e484e07790feb45629">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4bc7ff40-434e-4c6d-8428-0c665104b7a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="99b79b3d8b9bfdba0e64adc89a3cf448" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
-    <xsd:import namespace="5a827679-a132-4c88-bdb0-a978ce7a8b2d"/>
-    <xsd:import namespace="9921d756-3b1e-4e19-bd90-0d5dcbdf1ae1"/>
+    <xsd:import namespace="4bc7ff40-434e-4c6d-8428-0c665104b7a9"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:HasDigitalSignature" minOccurs="0"/>
+                <xsd:element ref="ns2:DigitalSignatureProvider" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
@@ -519,93 +513,69 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="8" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="14" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="9" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="15" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5a827679-a132-4c88-bdb0-a978ce7a8b2d" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4bc7ff40-434e-4c6d-8428-0c665104b7a9" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="12" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="13" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+    <xsd:element name="HasDigitalSignature" ma:index="11" nillable="true" ma:displayName="Signed electronically" ma:internalName="HasDigitalSignature" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DigitalSignatureProvider" ma:index="12" nillable="true" ma:displayName="Signature provider" ma:internalName="DigitalSignatureProvider" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceBillingMetadata" ma:index="14" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="13" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="e385fb40-52d4-4fae-9c5b-3e8ff8a5878e" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="19" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="20" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="21" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="22" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9921d756-3b1e-4e19-bd90-0d5dcbdf1ae1" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="17" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{5879a8a9-350e-4fc3-8a29-44adb29f3e41}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="9921d756-3b1e-4e19-bd90-0d5dcbdf1ae1">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -707,70 +677,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="9921d756-3b1e-4e19-bd90-0d5dcbdf1ae1" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5a827679-a132-4c88-bdb0-a978ce7a8b2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F30A48A-5017-4629-B011-16E35D752D71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="5a827679-a132-4c88-bdb0-a978ce7a8b2d"/>
-    <ds:schemaRef ds:uri="9921d756-3b1e-4e19-bd90-0d5dcbdf1ae1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F758571B-60A8-45A7-BD59-8D92C974AD35}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08206A00-993E-4B05-863B-F2B84DB98FF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08206A00-993E-4B05-863B-F2B84DB98FF6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F758571B-60A8-45A7-BD59-8D92C974AD35}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="9921d756-3b1e-4e19-bd90-0d5dcbdf1ae1"/>
-    <ds:schemaRef ds:uri="5a827679-a132-4c88-bdb0-a978ce7a8b2d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1363CAED-AD1E-4248-952C-7C02C79A45B5}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>